<commit_message>
Start v2 with numpy, minor v1 cleanups, updated benchmarks
</commit_message>
<xml_diff>
--- a/Perceptron Benchmarks.xlsx
+++ b/Perceptron Benchmarks.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>Nim</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>Numba</t>
+  </si>
+  <si>
+    <t>Macbook retina Python 3.4 64bity</t>
   </si>
 </sst>
 </file>
@@ -113,9 +116,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -125,11 +130,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="8">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -460,10 +467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -532,7 +539,7 @@
         <v>9.321266968325792E-2</v>
       </c>
       <c r="C4" s="1">
-        <f t="shared" ref="C4:H4" si="0">C3/$F$3</f>
+        <f t="shared" ref="C4:G4" si="0">C3/$F$3</f>
         <v>9.5776772247360489E-2</v>
       </c>
       <c r="D4" s="1">
@@ -593,6 +600,29 @@
       <c r="I9" s="1">
         <f>I8/$F$3</f>
         <v>0.92458521870286581</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="F12">
+        <v>7.32</v>
+      </c>
+      <c r="G12">
+        <v>4.01</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="F13" s="1">
+        <f t="shared" ref="F13:G13" si="2">F12/$F$3</f>
+        <v>1.1040723981900453</v>
+      </c>
+      <c r="G13" s="1">
+        <f t="shared" si="2"/>
+        <v>0.60482654600301655</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update benchmark result sheet.
</commit_message>
<xml_diff>
--- a/Perceptron Benchmarks.xlsx
+++ b/Perceptron Benchmarks.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>Nim</t>
   </si>
@@ -470,7 +470,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -608,21 +608,24 @@
       </c>
     </row>
     <row r="12" spans="1:10">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
       <c r="F12">
-        <v>7.32</v>
+        <v>6.66</v>
       </c>
       <c r="G12">
-        <v>4.01</v>
+        <v>3.15</v>
       </c>
     </row>
     <row r="13" spans="1:10">
       <c r="F13" s="1">
         <f t="shared" ref="F13:G13" si="2">F12/$F$3</f>
-        <v>1.1040723981900453</v>
+        <v>1.004524886877828</v>
       </c>
       <c r="G13" s="1">
-        <f t="shared" si="2"/>
-        <v>0.60482654600301655</v>
+        <f>G12/$F12</f>
+        <v>0.47297297297297297</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Re-arrange files. Re-write nim and julia versions. update benchmarks.
</commit_message>
<xml_diff>
--- a/Perceptron Benchmarks.xlsx
+++ b/Perceptron Benchmarks.xlsx
@@ -1,16 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10411"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lewislevin/Dropbox/Python-code/Benchmark_perceptron/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02C15432-EA59-8E4E-97AE-62201023671C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520" tabRatio="500"/>
+    <workbookView xWindow="6020" yWindow="6960" windowWidth="25600" windowHeight="15460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="results" sheetId="1" r:id="rId1"/>
+    <sheet name="machine specs" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -19,20 +35,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
   <si>
     <t>Nim</t>
   </si>
   <si>
-    <t>PyPy</t>
-  </si>
-  <si>
     <t>Cyth</t>
   </si>
   <si>
-    <t>Nui</t>
-  </si>
-  <si>
     <t>CPy</t>
   </si>
   <si>
@@ -58,12 +68,51 @@
   </si>
   <si>
     <t>Macbook retina Python 3.4 64bity</t>
+  </si>
+  <si>
+    <t>bign = 100</t>
+  </si>
+  <si>
+    <t>Nuitka</t>
+  </si>
+  <si>
+    <t>Julia via repl</t>
+  </si>
+  <si>
+    <t>Julia cmdline</t>
+  </si>
+  <si>
+    <t>PyPy cmdline</t>
+  </si>
+  <si>
+    <t>pypy ipython</t>
+  </si>
+  <si>
+    <t>Pct of Cpy</t>
+  </si>
+  <si>
+    <t>Cpy</t>
+  </si>
+  <si>
+    <t>Numpy</t>
+  </si>
+  <si>
+    <t>Numba Numpy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Numba </t>
+  </si>
+  <si>
+    <t>Julia repl</t>
+  </si>
+  <si>
+    <t>Mac iMac</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
@@ -116,9 +165,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="8">
+  <cellStyleXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -130,19 +185,509 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="8">
+  <cellStyles count="14">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="12" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>215900</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>749300</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1041400" y="635000"/>
+          <a:ext cx="3835400" cy="5638800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Model Name:	MacBook Pro</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>  Model Identifier:	MacBookPro11,1</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>  Processor Name:	Intel Core i5</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>  Processor Speed:	2.4 GHz</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>  Number of Processors:	1</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>  Total Number of Cores:	2</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="it-IT" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>  L2 Cache (per Core):	256 KB</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>  L3 Cache:	3 MB</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>  Memory:	8 GB</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="de-DE" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Apple SSD Controller:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" b="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>  Vendor:	Apple</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>  Product:	SSD Controller</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>  Physical Interconnect:	PCI</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>  Link Width:	x2</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>  Link Speed:	5.0 GT/s</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>  Description:	AHCI Version 1.30 Supported</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" b="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>APPLE SSD SM0256F:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" b="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>  Capacity:	251 GB (251,000,193,024 bytes)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>  Model:	APPLE SSD SM0256F                       </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>  Revision:	UXM2JA1Q</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>  Serial Number:	S1K4NYADB63005      </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>  Native Command Queuing:	Yes</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>  Queue Depth:	32</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>  Removable Media:	No</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>  Detachable Drive:	No</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>  BSD Name:	disk0</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>  Medium Type:	Solid State</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>  TRIM Support:	Yes</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -466,52 +1011,64 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="8" max="8" width="14" customWidth="1"/>
+    <col min="9" max="9" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>0</v>
       </c>
       <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" t="s">
+      <c r="H2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>3</v>
-      </c>
-      <c r="F2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" t="s">
-        <v>5</v>
       </c>
       <c r="B3">
         <v>0.61799999999999999</v>
@@ -519,122 +1076,261 @@
       <c r="C3">
         <v>0.63500000000000001</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>1.53</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>5.0590000000000002</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>6.63</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <f>1*60+15</f>
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B4" s="1">
-        <f>B3/$F$3</f>
+        <f>B3/$G$3</f>
         <v>9.321266968325792E-2</v>
       </c>
       <c r="C4" s="1">
-        <f t="shared" ref="C4:G4" si="0">C3/$F$3</f>
+        <f t="shared" ref="C4:H4" si="0">C3/$G$3</f>
         <v>9.5776772247360489E-2</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="1"/>
+      <c r="E4" s="1">
         <f t="shared" si="0"/>
         <v>0.23076923076923078</v>
       </c>
-      <c r="E4" s="1">
+      <c r="F4" s="1">
         <f t="shared" si="0"/>
         <v>0.76304675716440429</v>
       </c>
-      <c r="F4" s="1">
+      <c r="G4" s="1">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G4" s="1">
+      <c r="H4" s="1">
         <f t="shared" si="0"/>
         <v>11.312217194570136</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F8">
+        <v>3</v>
+      </c>
+      <c r="B7">
+        <v>0.65400000000000003</v>
+      </c>
+      <c r="C7">
+        <v>0.61299999999999999</v>
+      </c>
+      <c r="F7">
+        <v>4.5960000000000001</v>
+      </c>
+      <c r="G7">
+        <v>6.3</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B8" s="1">
+        <f>B7/$G$7</f>
+        <v>0.10380952380952381</v>
+      </c>
+      <c r="C8" s="1">
+        <f>C7/$G$7</f>
+        <v>9.7301587301587306E-2</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="F8" s="1">
+        <f>F7/$G$7</f>
+        <v>0.72952380952380957</v>
+      </c>
+      <c r="G8" s="1">
+        <f>G7/$G$7</f>
+        <v>1</v>
+      </c>
+      <c r="H8" s="1">
+        <f>H7/$G$7</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>0</v>
+      </c>
+      <c r="K11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B12">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="K12">
+        <v>5.1999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18">
+        <v>0.65</v>
+      </c>
+      <c r="C18" s="1">
+        <f>B18/$B$23</f>
+        <v>0.10761589403973511</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19">
+        <v>0.56299999999999994</v>
+      </c>
+      <c r="C19" s="1">
+        <f>B19/$B$23</f>
+        <v>9.3211920529801318E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20">
+        <v>0.55400000000000005</v>
+      </c>
+      <c r="C20" s="1">
+        <f>B20/$B$23</f>
+        <v>9.1721854304635766E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23">
         <v>6.04</v>
       </c>
-      <c r="G8">
+      <c r="C23" s="1">
+        <f t="shared" ref="C23:C28" si="1">B23/$B$23</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24">
         <v>32</v>
       </c>
-      <c r="H8">
+      <c r="C24" s="1">
+        <f t="shared" si="1"/>
+        <v>5.298013245033113</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>20</v>
+      </c>
+      <c r="B25">
         <v>21.2</v>
       </c>
-      <c r="I8">
+      <c r="C25" s="1">
+        <f t="shared" si="1"/>
+        <v>3.5099337748344368</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>21</v>
+      </c>
+      <c r="B26">
         <v>6.13</v>
       </c>
-      <c r="J8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="F9" s="1">
-        <f t="shared" ref="F9:G9" si="1">F8/$F$3</f>
-        <v>0.91101055806938158</v>
-      </c>
-      <c r="G9" s="1">
+      <c r="C26" s="1">
         <f t="shared" si="1"/>
-        <v>4.826546003016591</v>
-      </c>
-      <c r="H9" s="1">
-        <f>H8/$F$3</f>
-        <v>3.1975867269984914</v>
-      </c>
-      <c r="I9" s="1">
-        <f>I8/$F$3</f>
-        <v>0.92458521870286581</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
-      <c r="A12" t="s">
-        <v>5</v>
-      </c>
-      <c r="F12">
-        <v>6.66</v>
-      </c>
-      <c r="G12">
-        <v>3.15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10">
-      <c r="F13" s="1">
-        <f t="shared" ref="F13:G13" si="2">F12/$F$3</f>
-        <v>1.004524886877828</v>
-      </c>
-      <c r="G13" s="1">
-        <f>G12/$F12</f>
-        <v>0.47297297297297297</v>
+        <v>1.0149006622516556</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="C27" s="1">
+        <f t="shared" si="1"/>
+        <v>1.4072847682119206E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>14</v>
+      </c>
+      <c r="B28">
+        <v>0.69</v>
+      </c>
+      <c r="C28" s="1">
+        <f t="shared" si="1"/>
+        <v>0.11423841059602648</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>